<commit_message>
Create Demo Board PIC24
</commit_message>
<xml_diff>
--- a/Elec/2011/Balises IR/Commande Farnell 2.xlsx
+++ b/Elec/2011/Balises IR/Commande Farnell 2.xlsx
@@ -253,7 +253,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -295,8 +295,15 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -307,6 +314,18 @@
       <patternFill patternType="solid">
         <fgColor theme="1"/>
         <bgColor theme="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -361,7 +380,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -406,6 +425,10 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -588,66 +611,6 @@
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <bottom style="medium">
-          <color theme="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="medium">
-          <color theme="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="1"/>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -720,6 +683,66 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="medium">
+          <color theme="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color theme="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="1"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
@@ -773,15 +796,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A10:F47" totalsRowCount="1" headerRowDxfId="9" dataDxfId="8" headerRowBorderDxfId="6" tableBorderDxfId="7" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A10:F47" totalsRowCount="1" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12" dataCellStyle="Normal">
   <autoFilter ref="A10:F46"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Comment" dataDxfId="15" totalsRowDxfId="5" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="Pattern" dataDxfId="14" totalsRowDxfId="4" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Quantity" dataDxfId="13" totalsRowDxfId="3" dataCellStyle="Normal"/>
-    <tableColumn id="5" name="Ref farnell" dataDxfId="12" totalsRowDxfId="2" dataCellStyle="Normal"/>
-    <tableColumn id="6" name="PU (HT)" dataDxfId="11" totalsRowDxfId="1" dataCellStyle="Normal"/>
-    <tableColumn id="8" name="Prix (€ - HT)" totalsRowFunction="custom" dataDxfId="10" totalsRowDxfId="0" dataCellStyle="Normal">
+    <tableColumn id="1" name="Comment" dataDxfId="11" totalsRowDxfId="5" dataCellStyle="Normal"/>
+    <tableColumn id="2" name="Pattern" dataDxfId="10" totalsRowDxfId="4" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="Quantity" dataDxfId="9" totalsRowDxfId="3" dataCellStyle="Normal"/>
+    <tableColumn id="5" name="Ref farnell" dataDxfId="8" totalsRowDxfId="2" dataCellStyle="Normal"/>
+    <tableColumn id="6" name="PU (HT)" dataDxfId="7" totalsRowDxfId="1" dataCellStyle="Normal"/>
+    <tableColumn id="8" name="Prix (€ - HT)" totalsRowFunction="custom" dataDxfId="6" totalsRowDxfId="0" dataCellStyle="Normal">
       <calculatedColumnFormula>Tableau1[[#This Row],[Quantity]]*Tableau1[[#This Row],[PU (HT)]]</calculatedColumnFormula>
       <totalsRowFormula>SUM([Prix (€ - HT)])</totalsRowFormula>
     </tableColumn>
@@ -1077,8 +1100,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A4:J67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1164,7 +1187,7 @@
         <f>Tableau1[[#This Row],[Quantity]]*Tableau1[[#This Row],[PU (HT)]]</f>
         <v>20.32</v>
       </c>
-      <c r="H11" s="3"/>
+      <c r="H11" s="26"/>
       <c r="I11" s="2"/>
       <c r="J11" s="3"/>
     </row>
@@ -1188,7 +1211,7 @@
         <f>Tableau1[[#This Row],[Quantity]]*Tableau1[[#This Row],[PU (HT)]]</f>
         <v>18.559999999999999</v>
       </c>
-      <c r="H12" s="3"/>
+      <c r="H12" s="26"/>
       <c r="I12" s="2"/>
       <c r="J12" s="3"/>
     </row>
@@ -1404,7 +1427,7 @@
         <f>Tableau1[[#This Row],[Quantity]]*Tableau1[[#This Row],[PU (HT)]]</f>
         <v>8.75</v>
       </c>
-      <c r="H21" s="3"/>
+      <c r="H21" s="26"/>
       <c r="I21" s="2"/>
       <c r="J21" s="3"/>
     </row>
@@ -1716,6 +1739,7 @@
         <f>Tableau1[[#This Row],[Quantity]]*Tableau1[[#This Row],[PU (HT)]]</f>
         <v>11.7</v>
       </c>
+      <c r="H34" s="25"/>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="18" t="s">
@@ -1737,6 +1761,7 @@
         <f>Tableau1[[#This Row],[Quantity]]*Tableau1[[#This Row],[PU (HT)]]</f>
         <v>1.1299999999999999</v>
       </c>
+      <c r="H35" s="27"/>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" t="s">
@@ -1758,6 +1783,7 @@
         <f>Tableau1[[#This Row],[Quantity]]*Tableau1[[#This Row],[PU (HT)]]</f>
         <v>2.86</v>
       </c>
+      <c r="H36" s="27"/>
     </row>
     <row r="37" spans="1:10" ht="15" customHeight="1">
       <c r="A37" t="s">
@@ -1779,6 +1805,7 @@
         <f>Tableau1[[#This Row],[Quantity]]*Tableau1[[#This Row],[PU (HT)]]</f>
         <v>9.68</v>
       </c>
+      <c r="H37" s="27"/>
     </row>
     <row r="38" spans="1:10" ht="15" customHeight="1">
       <c r="A38" t="s">
@@ -1800,6 +1827,7 @@
         <f>Tableau1[[#This Row],[Quantity]]*Tableau1[[#This Row],[PU (HT)]]</f>
         <v>49.8</v>
       </c>
+      <c r="H38" s="24"/>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="18" t="s">
@@ -1821,6 +1849,7 @@
         <f>Tableau1[[#This Row],[Quantity]]*Tableau1[[#This Row],[PU (HT)]]</f>
         <v>6.26</v>
       </c>
+      <c r="H39" s="27"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="18" t="s">
@@ -1842,6 +1871,7 @@
         <f>Tableau1[[#This Row],[Quantity]]*Tableau1[[#This Row],[PU (HT)]]</f>
         <v>4.4800000000000004</v>
       </c>
+      <c r="H40" s="27"/>
     </row>
     <row r="41" spans="1:10">
       <c r="A41" s="18" t="s">
@@ -1905,6 +1935,7 @@
         <f>Tableau1[[#This Row],[Quantity]]*Tableau1[[#This Row],[PU (HT)]]</f>
         <v>4.26</v>
       </c>
+      <c r="H43" s="27"/>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="18" t="s">
@@ -1926,6 +1957,7 @@
         <f>Tableau1[[#This Row],[Quantity]]*Tableau1[[#This Row],[PU (HT)]]</f>
         <v>5.88</v>
       </c>
+      <c r="H44" s="27"/>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="15" t="s">

</xml_diff>